<commit_message>
feat: Criação do projeto.
</commit_message>
<xml_diff>
--- a/src/data/modelo.xlsx
+++ b/src/data/modelo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27990" windowHeight="12930"/>
+    <workbookView windowWidth="27930" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="FREQUÊNCIA" sheetId="1" r:id="rId1"/>
@@ -226,10 +226,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -318,23 +318,129 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Times New Roman"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Times New Roman"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -348,117 +454,11 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Times New Roman"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Times New Roman"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="40">
     <fill>
@@ -511,19 +511,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -535,7 +619,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -547,151 +643,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -903,21 +903,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -957,13 +942,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -972,6 +961,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1003,152 +1003,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="30" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1216,9 +1216,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1329,7 +1326,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5299075" y="104775"/>
+          <a:off x="4749800" y="104775"/>
           <a:ext cx="1743075" cy="504825"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1543,11 +1540,11 @@
   <sheetPr/>
   <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4416666666667" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.4380952380952" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="15.6666666666667" customWidth="1"/>
@@ -1692,9 +1689,9 @@
       <c r="H13" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" ht="19.5" customHeight="1" spans="1:11">
       <c r="A14" s="9">
@@ -1713,11 +1710,11 @@
       <c r="H14" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="28"/>
+      <c r="I14" s="27"/>
       <c r="J14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="K14" s="29"/>
+      <c r="K14" s="28"/>
     </row>
     <row r="15" ht="19.5" customHeight="1" spans="1:5">
       <c r="A15" s="9">
@@ -1751,9 +1748,9 @@
       <c r="H16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17" ht="19.5" customHeight="1" spans="1:11">
       <c r="A17" s="9">
@@ -1769,12 +1766,12 @@
         <v>19</v>
       </c>
       <c r="E17" s="21"/>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="31"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
     </row>
     <row r="18" ht="19.5" customHeight="1" spans="1:5">
       <c r="A18" s="9">
@@ -2023,12 +2020,12 @@
         <v>26</v>
       </c>
       <c r="D37" s="18"/>
-      <c r="E37" s="25"/>
+      <c r="E37" s="24"/>
     </row>
     <row r="38" ht="57.75" customHeight="1" spans="3:5">
       <c r="C38" s="19"/>
       <c r="D38" s="18"/>
-      <c r="E38" s="25"/>
+      <c r="E38" s="24"/>
     </row>
     <row r="39" ht="12.75" customHeight="1"/>
     <row r="40" ht="12.75" customHeight="1"/>

</xml_diff>

<commit_message>
feat: Adiciona campos de horário de início e fim na geração de planilhas, implementa validações e refatora componentes para melhor gerenciamento de dados de horário
</commit_message>
<xml_diff>
--- a/src/data/modelo.xlsx
+++ b/src/data/modelo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
   <si>
     <t>JP CORPO E MENTE LTDA
 CNPJ: 49.317.168/0001-14
@@ -168,6 +168,9 @@
     <t>COMPETENCIA</t>
   </si>
   <si>
+    <t>HORÁRIO</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -197,10 +200,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="32">
     <font>
@@ -297,9 +300,123 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -312,125 +429,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="40">
     <fill>
@@ -483,187 +486,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,11 +878,56 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -901,54 +949,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -964,10 +969,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -975,142 +978,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1120,7 +1123,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1178,9 +1181,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1496,7 +1496,7 @@
   <dimension ref="A1:K1010"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4333333333333" defaultRowHeight="15" customHeight="1"/>
@@ -1627,9 +1627,9 @@
       <c r="H13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="27"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="26"/>
     </row>
     <row r="14" ht="19.5" customHeight="1" spans="1:11">
       <c r="A14" s="10">
@@ -1642,9 +1642,9 @@
       </c>
       <c r="E14" s="21"/>
       <c r="H14" s="23"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="28"/>
     </row>
     <row r="15" ht="19.5" customHeight="1" spans="1:5">
       <c r="A15" s="10">
@@ -1670,9 +1670,9 @@
       <c r="H16" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="27"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="26"/>
     </row>
     <row r="17" ht="19.5" customHeight="1" spans="1:11">
       <c r="A17" s="10">
@@ -1684,10 +1684,10 @@
         <v>13</v>
       </c>
       <c r="E17" s="21"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="31"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="30"/>
     </row>
     <row r="18" ht="19.5" customHeight="1" spans="1:5">
       <c r="A18" s="10">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="E18" s="21"/>
     </row>
-    <row r="19" ht="19.5" customHeight="1" spans="1:5">
+    <row r="19" ht="19.5" customHeight="1" spans="1:11">
       <c r="A19" s="10">
         <v>8</v>
       </c>
@@ -1710,8 +1710,14 @@
         <v>13</v>
       </c>
       <c r="E19" s="21"/>
-    </row>
-    <row r="20" ht="19.5" customHeight="1" spans="1:5">
+      <c r="H19" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
+    </row>
+    <row r="20" ht="19.5" customHeight="1" spans="1:11">
       <c r="A20" s="10">
         <v>9</v>
       </c>
@@ -1721,6 +1727,10 @@
         <v>13</v>
       </c>
       <c r="E20" s="21"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="28"/>
     </row>
     <row r="21" ht="19.5" customHeight="1" spans="1:5">
       <c r="A21" s="10">
@@ -1971,7 +1981,7 @@
     </row>
     <row r="44" ht="19.5" customHeight="1" spans="1:3">
       <c r="A44" s="15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B44" s="16"/>
       <c r="C44" s="17">
@@ -1983,15 +1993,15 @@
     <row r="46" ht="19.5" customHeight="1"/>
     <row r="47" ht="19.5" customHeight="1" spans="3:5">
       <c r="C47" s="18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D47" s="19"/>
-      <c r="E47" s="25"/>
+      <c r="E47" s="24"/>
     </row>
     <row r="48" ht="57.75" customHeight="1" spans="3:5">
       <c r="C48" s="20"/>
       <c r="D48" s="19"/>
-      <c r="E48" s="25"/>
+      <c r="E48" s="24"/>
     </row>
     <row r="49" ht="12.75" customHeight="1"/>
     <row r="50" ht="12.75" customHeight="1"/>
@@ -2956,7 +2966,7 @@
     <row r="1009" ht="15.75" customHeight="1"/>
     <row r="1010" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="23">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:B3"/>
@@ -2975,6 +2985,8 @@
     <mergeCell ref="H14:K14"/>
     <mergeCell ref="H16:K16"/>
     <mergeCell ref="H17:K17"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="C47:E47"/>
     <mergeCell ref="C48:E48"/>

</xml_diff>